<commit_message>
vault backup: 2024-07-11 20:58:23
Affected files:
.obsidian/workspace.json
assest/20240626-解放项目-语音指令表-v1.0.1.xlsx
</commit_message>
<xml_diff>
--- a/assest/20240626-解放项目-语音指令表-v1.0.1.xlsx
+++ b/assest/20240626-解放项目-语音指令表-v1.0.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9180" activeTab="3"/>
+    <workbookView windowWidth="16331" windowHeight="9180" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="变更记录" sheetId="19" r:id="rId1"/>
@@ -30074,9 +30074,9 @@
   <dimension ref="A1:X200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>

</xml_diff>

<commit_message>
vault backup: 2024-07-24 12:18:44
Affected files:
.obsidian/workspace.json
assest/20240426-航天青岛一汽项目-项目标准需求协议表.xlsx
assest/20240626-解放项目-语音指令表-v1.0.1.xlsx
assest/20240626-解放项目-问题反馈.xlsx
assest/dongfeng/TTSSERVICE 使用说明.docx
assest/dongfeng/TTSSERVICE.apk
assest/dongfeng/TTSSample.zip
assest/dongfeng/dongfeng_structured.json
assest/dongfeng/res_txz_adapter_cmd_keywords.json
assest/dongfeng/resume.json
assest/陕汽德龙x6000英文指令表20240715.xlsx
log/2024-07-23.md
</commit_message>
<xml_diff>
--- a/assest/20240626-解放项目-语音指令表-v1.0.1.xlsx
+++ b/assest/20240626-解放项目-语音指令表-v1.0.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9060" firstSheet="2" activeTab="6"/>
+    <workbookView windowWidth="22188" windowHeight="9060" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="变更记录" sheetId="19" r:id="rId1"/>
@@ -30046,9 +30046,9 @@
   <dimension ref="A1:X200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -35655,7 +35655,7 @@
   <dimension ref="A1:AC189"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
@@ -42490,10 +42490,10 @@
   <sheetPr/>
   <dimension ref="A1:X199"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -48057,10 +48057,10 @@
   <sheetPr/>
   <dimension ref="A1:X95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>

</xml_diff>